<commit_message>
finish first submitted version
</commit_message>
<xml_diff>
--- a/FIGS/tables.xlsx
+++ b/FIGS/tables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TAB1_prevalence_cfr15year_BR" sheetId="1" state="visible" r:id="rId2"/>
@@ -341,7 +341,7 @@
     <t xml:space="preserve">TABLE 2: Educational pairings prevalence rates and cohort fertility rates for female cohorts born in 1925-39, 1940-54 and 1955-69 for Brazil and selected regions. Source: Brazilian National Censuses, 1970-2010.</t>
   </si>
   <si>
-    <t xml:space="preserve">Central-West</t>
+    <t xml:space="preserve">Midwest</t>
   </si>
   <si>
     <t xml:space="preserve">83.70</t>
@@ -1507,7 +1507,7 @@
   </sheetPr>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -2069,7 +2069,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2171,7 +2171,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B5" s="0" t="s">
@@ -2200,7 +2200,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B6" s="0" t="s">
@@ -2229,7 +2229,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B7" s="0" t="s">
@@ -2258,7 +2258,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B8" s="0" t="s">
@@ -2287,7 +2287,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B9" s="0" t="s">
@@ -2316,7 +2316,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B10" s="0" t="s">
@@ -2345,7 +2345,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B11" s="0" t="s">
@@ -2374,7 +2374,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B12" s="0" t="s">
@@ -2403,7 +2403,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B13" s="0" t="s">
@@ -2432,7 +2432,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B14" s="0" t="s">
@@ -2461,7 +2461,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B15" s="0" t="s">
@@ -2490,7 +2490,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B16" s="0" t="s">
@@ -2519,7 +2519,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B17" s="0" t="s">
@@ -2548,7 +2548,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B18" s="0" t="s">
@@ -2577,7 +2577,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B19" s="15" t="s">
@@ -3751,8 +3751,8 @@
   </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>